<commit_message>
Adding new file and making carousel
</commit_message>
<xml_diff>
--- a/CompunetCbte/ExcelTemplate/CbteQuestionUpload.xlsx
+++ b/CompunetCbte/ExcelTemplate/CbteQuestionUpload.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Course Code</t>
   </si>
@@ -81,13 +81,49 @@
   </si>
   <si>
     <t>PRE-DEGREE</t>
+  </si>
+  <si>
+    <t>627 + 183</t>
+  </si>
+  <si>
+    <t>Write 3.75 million in figures.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>20 – 3 × 5</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>BlankChoice</t>
+  </si>
+  <si>
+    <t>Don’t inlude "only"</t>
+  </si>
+  <si>
+    <t>The value of x + x(xx) when x = 2 is</t>
+  </si>
+  <si>
+    <t>Round 36,993 to the nearest thousands</t>
+  </si>
+  <si>
+    <t>Round 6.724 to the nearest hundredth</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +137,30 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF646464"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -124,9 +184,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,6 +212,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B21CD6-01C3-4211-A264-91C03C1C28EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5943600" y="1800225"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,17 +571,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -554,8 +684,201 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>810</v>
+      </c>
+      <c r="E4">
+        <v>815</v>
+      </c>
+      <c r="F4">
+        <v>825</v>
+      </c>
+      <c r="G4">
+        <v>821</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3750000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>85</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>36000</v>
+      </c>
+      <c r="E8">
+        <v>36900</v>
+      </c>
+      <c r="F8">
+        <v>40000</v>
+      </c>
+      <c r="G8">
+        <v>36950</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>6750</v>
+      </c>
+      <c r="E9">
+        <v>6000</v>
+      </c>
+      <c r="F9">
+        <v>7000</v>
+      </c>
+      <c r="G9">
+        <v>6700</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>